<commit_message>
Dev 20012024 (Post pre-go-live workshop)
</commit_message>
<xml_diff>
--- a/config/forms/contact/cases_group-create.xlsx
+++ b/config/forms/contact/cases_group-create.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\morlig\icap\dmi-adam-repositories\dmi-adam\config\forms\contact\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37696524-DFE9-4E06-AA12-920924320024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AB8018-601D-4DE8-9B86-A12AF99541C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7807" uniqueCount="1990">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7862" uniqueCount="2005">
   <si>
     <t>type</t>
   </si>
@@ -6001,20 +6001,65 @@
     <t>../../cases_group/outbreak_location/name</t>
   </si>
   <si>
-    <t>&lt;h4 style="border-bottom: rgb(150, 150, 150) dashed 1px; padding: 15px 0"&gt;Outbreak Location: ${outbreak_location_name}&lt;/h4&gt;</t>
-  </si>
-  <si>
     <t>hidden select-contact type-outbreak_location</t>
   </si>
   <si>
-    <t>&lt;h4 style="border-bottom: rgb(150, 150, 150) dashed 1px; padding: 15px 0"&gt;Outbreak: ${outbreak_name}&lt;/h4&gt;</t>
+    <t>person</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>meta</t>
+  </si>
+  <si>
+    <t>A primary contact associated with this &lt;strong&gt;cases group&lt;/strong&gt; will be automatically created.</t>
+  </si>
+  <si>
+    <t>init</t>
+  </si>
+  <si>
+    <t>select_one contact</t>
+  </si>
+  <si>
+    <t>create_new_person</t>
+  </si>
+  <si>
+    <t>Set the Primary Contact</t>
+  </si>
+  <si>
+    <t>db:person</t>
+  </si>
+  <si>
+    <t>select_person</t>
+  </si>
+  <si>
+    <t>Select the Primary Contact</t>
+  </si>
+  <si>
+    <t>selected(${create_new_person},'old_person')</t>
+  </si>
+  <si>
+    <t>db-object</t>
+  </si>
+  <si>
+    <t>concat(../../cases_group/name, " - Primary Contact")</t>
+  </si>
+  <si>
+    <t>coalesce(${select_person},"NEW")</t>
+  </si>
+  <si>
+    <t>&lt;h4 style="font-weight: normal; border-bottom: rgb(150, 150, 150) dashed 1px; padding: 15px 0"&gt;Outbreak: ${outbreak_name}&lt;/h4&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h4 style="font-weight: normal; border-bottom: rgb(150, 150, 150) dashed 1px; padding: 15px 0"&gt;Outbreak Location: ${outbreak_location_name}&lt;/h4&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="64"/>
@@ -6053,8 +6098,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6091,8 +6143,13 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -6100,16 +6157,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6131,14 +6198,19 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
     <cellStyle name="40% - Accent2" xfId="4" builtinId="35"/>
     <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
     <cellStyle name="60% - Accent3" xfId="5" builtinId="40"/>
+    <cellStyle name="Accent6" xfId="6" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6364,14 +6436,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N965"/>
+  <dimension ref="A1:Z984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C2" sqref="C2"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -6395,7 +6467,7 @@
     <col min="27" max="32" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6439,7 +6511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
@@ -6454,7 +6526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
@@ -6465,7 +6537,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -6479,7 +6551,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -6493,7 +6565,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -6507,23 +6579,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:26" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>1968</v>
+        <v>1992</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>16</v>
@@ -6532,301 +6604,528 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>1993</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1994</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>1995</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
+      <c r="G11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5" t="s">
+        <v>1965</v>
+      </c>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+    </row>
+    <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>1996</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>1997</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1998</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1999</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>2000</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+    </row>
+    <row r="13" spans="1:26" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:26" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>1966</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="17" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B17" t="s">
         <v>0</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M17" t="s">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1964</v>
+      </c>
+      <c r="J18" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1989</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:13" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>1990</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:13" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>1968</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="C28" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="M29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="M30" t="s">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B31" t="s">
         <v>1979</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C31" t="s">
         <v>16</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J31" t="s">
         <v>1978</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="32" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B32" t="s">
         <v>1980</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C32" t="s">
         <v>16</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J32" t="s">
         <v>1981</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="33" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B33" t="s">
         <v>1983</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C33" t="s">
         <v>16</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J33" t="s">
         <v>1986</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:10" s="12" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
+    <row r="34" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="1:10" s="12" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="12" t="s">
         <v>1982</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B35" s="12" t="s">
         <v>1984</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>1989</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="12" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+      <c r="C35" s="17" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="12" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="12" t="s">
         <v>1982</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B36" s="12" t="s">
         <v>1985</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C36" s="17" t="s">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:10" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>1975</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="11" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>1971</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>1976</v>
+      </c>
+      <c r="F39" s="11" t="s">
         <v>1987</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:10" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+      <c r="G39" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="11" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:10" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B42" s="10" t="s">
+        <v>1970</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="11" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="11" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>1973</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>1975</v>
       </c>
-      <c r="C20" s="10" t="s">
+    </row>
+    <row r="47" spans="1:10" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1977</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+      <c r="I48" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>1966</v>
+      </c>
+      <c r="J49" s="16" t="s">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="51" spans="1:10" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>1963</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="11" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>1971</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>1976</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>1988</v>
-      </c>
-      <c r="G21" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>1972</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="11" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+      <c r="F51" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>1969</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:10" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>1970</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="11" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>1969</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="11" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>1973</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>1974</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
+    </row>
+    <row r="52" spans="1:10" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J52" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J53" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J54" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>1970</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
+    </row>
+    <row r="56" spans="1:10" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>1975</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1977</v>
-      </c>
-      <c r="D30" t="s">
-        <v>26</v>
-      </c>
-      <c r="I30" t="s">
-        <v>1964</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:10" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>1963</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -7728,6 +8027,25 @@
     <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -36583,7 +36901,7 @@
       </c>
       <c r="C2" s="4" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-11-28 12-33</v>
+        <v>2024-01-20 11-14</v>
       </c>
       <c r="D2" t="s">
         <v>47</v>

</xml_diff>